<commit_message>
Till negative test cases
</commit_message>
<xml_diff>
--- a/MainAssignment-api testing/src/test/resources/user data.xlsx
+++ b/MainAssignment-api testing/src/test/resources/user data.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdhurwe\Documents\MainAssignment-api testing\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdhurwe\Documents\API testing\MainAssignment-api testing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD128C6-5EB7-4119-B09F-F93DA47A89B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EE9097-54A9-429C-B246-A5D3025EE917}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -58,14 +59,76 @@
   </si>
   <si>
     <t>6249e5a716a74e0017461657</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>TaskNum1</t>
+  </si>
+  <si>
+    <t>TaskNum2</t>
+  </si>
+  <si>
+    <t>TaskNum3</t>
+  </si>
+  <si>
+    <t>TaskNum4</t>
+  </si>
+  <si>
+    <t>TaskNum5</t>
+  </si>
+  <si>
+    <t>TaskNum6</t>
+  </si>
+  <si>
+    <t>TaskNum7</t>
+  </si>
+  <si>
+    <t>TaskNum8</t>
+  </si>
+  <si>
+    <t>TaskNum9</t>
+  </si>
+  <si>
+    <t>TaskNum10</t>
+  </si>
+  <si>
+    <t>TaskNum11</t>
+  </si>
+  <si>
+    <t>TaskNum12</t>
+  </si>
+  <si>
+    <t>TaskNum13</t>
+  </si>
+  <si>
+    <t>TaskNum14</t>
+  </si>
+  <si>
+    <t>TaskNum15</t>
+  </si>
+  <si>
+    <t>TaskNum16</t>
+  </si>
+  <si>
+    <t>TaskNum17</t>
+  </si>
+  <si>
+    <t>TaskNum18</t>
+  </si>
+  <si>
+    <t>TaskNum19</t>
+  </si>
+  <si>
+    <t>TaskNum20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +140,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -389,7 +458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -442,4 +511,129 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93B35E9-E3B6-48E0-848E-CED94434498F}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>